<commit_message>
Create graphs for frequency - ex1
</commit_message>
<xml_diff>
--- a/csv_out/topiccing/topiccing_discrimination_comparison_using_grouped_words.xlsx
+++ b/csv_out/topiccing/topiccing_discrimination_comparison_using_grouped_words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\IMF_VE_News\csv_out\topiccing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{19CCA1DA-606B-49EB-A068-733F938ACFCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0BAB61-D94F-4126-B601-5416633EA745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topiccing_discrimination_compar" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -623,17 +623,8 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -649,6 +640,15 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1003,11 +1003,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:AH53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,263 +1018,263 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="4" t="s">
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="4" t="s">
+      <c r="P2" s="22"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="4" t="s">
+      <c r="S2" s="22"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="8"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="4" t="s">
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="8" t="s">
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="4" t="s">
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="5"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="23"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="V3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="W3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="Z3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AA3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="AB3" t="s">
         <v>11</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AC3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AD3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AE3" s="9" t="s">
+      <c r="AE3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AF3" s="7" t="s">
+      <c r="AF3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="13"/>
+    <row r="4" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="10"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
-        <v>0</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
-        <v>0</v>
-      </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17">
-        <v>0</v>
-      </c>
-      <c r="L5" s="15">
-        <v>0</v>
-      </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="17">
-        <v>0</v>
-      </c>
-      <c r="O5" s="15">
-        <v>0</v>
-      </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="17">
-        <v>0</v>
-      </c>
-      <c r="R5" s="15">
-        <v>0</v>
-      </c>
-      <c r="S5" s="16"/>
-      <c r="T5" s="17">
-        <v>0</v>
-      </c>
-      <c r="U5" s="15">
-        <v>0</v>
-      </c>
-      <c r="V5" s="16"/>
-      <c r="W5" s="17">
-        <v>0</v>
-      </c>
-      <c r="X5" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="17">
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="12">
+        <v>0</v>
+      </c>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14">
+        <v>0</v>
+      </c>
+      <c r="U5" s="12">
+        <v>0</v>
+      </c>
+      <c r="V5" s="13"/>
+      <c r="W5" s="14">
+        <v>0</v>
+      </c>
+      <c r="X5" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1282,94 +1282,94 @@
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="15">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16">
-        <v>0</v>
-      </c>
-      <c r="E6" s="17">
-        <v>0</v>
-      </c>
-      <c r="F6" s="15">
-        <v>0</v>
-      </c>
-      <c r="G6" s="16">
-        <v>0</v>
-      </c>
-      <c r="H6" s="17">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16">
-        <v>0</v>
-      </c>
-      <c r="K6" s="17">
-        <v>0</v>
-      </c>
-      <c r="L6" s="15">
-        <v>0</v>
-      </c>
-      <c r="M6" s="16">
-        <v>0</v>
-      </c>
-      <c r="N6" s="17">
-        <v>0</v>
-      </c>
-      <c r="O6" s="15">
-        <v>0</v>
-      </c>
-      <c r="P6" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="17">
-        <v>0</v>
-      </c>
-      <c r="R6" s="15">
-        <v>0</v>
-      </c>
-      <c r="S6" s="16">
-        <v>0</v>
-      </c>
-      <c r="T6" s="17">
-        <v>0</v>
-      </c>
-      <c r="U6" s="15">
-        <v>0</v>
-      </c>
-      <c r="V6" s="16">
-        <v>0</v>
-      </c>
-      <c r="W6" s="17">
-        <v>0</v>
-      </c>
-      <c r="X6" s="15">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="16">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="15">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="16">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="17">
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="14">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0</v>
+      </c>
+      <c r="S6" s="13">
+        <v>0</v>
+      </c>
+      <c r="T6" s="14">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12">
+        <v>0</v>
+      </c>
+      <c r="V6" s="13">
+        <v>0</v>
+      </c>
+      <c r="W6" s="14">
+        <v>0</v>
+      </c>
+      <c r="X6" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="13">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -1377,94 +1377,94 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>0.1</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>3.5714285714285698E-2</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>7.3529411764705802E-2</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <v>0.30769230769230699</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="13">
         <v>0.16666666666666599</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="14">
         <v>0.26315789473684198</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="12">
         <v>0.1</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="13">
         <v>5.8823529411764698E-2</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="14">
         <v>8.7719298245614002E-2</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="12">
         <v>0.25</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="13">
         <v>0.107142857142857</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="14">
         <v>0.197368421052631</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="12">
         <v>0.33333333333333298</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="13">
         <v>0.12121212121212099</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="14">
         <v>0.24691358024691301</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="13">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="14">
         <v>0.14285714285714199</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V7" s="13">
         <v>0.11111111111111099</v>
       </c>
-      <c r="W7" s="17">
+      <c r="W7" s="14">
         <v>0.16129032258064499</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="12">
         <v>0.1</v>
       </c>
-      <c r="Y7" s="16">
+      <c r="Y7" s="13">
         <v>5.8823529411764698E-2</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="Z7" s="14">
         <v>8.7719298245614002E-2</v>
       </c>
-      <c r="AA7" s="18">
+      <c r="AA7" s="15">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AB7" s="18">
+      <c r="AB7" s="15">
         <v>0.11764705882352899</v>
       </c>
-      <c r="AC7" s="18">
+      <c r="AC7" s="15">
         <v>0.16393442622950799</v>
       </c>
-      <c r="AD7" s="15">
+      <c r="AD7" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AE7" s="16">
+      <c r="AE7" s="13">
         <v>0.11111111111111099</v>
       </c>
-      <c r="AF7" s="17">
+      <c r="AF7" s="14">
         <v>0.16129032258064499</v>
       </c>
     </row>
@@ -1472,94 +1472,94 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>0.38461538461538403</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>0.12195121951219499</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>0.26881720430107497</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <v>0.5</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="13">
         <v>0.21621621621621601</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="14">
         <v>0.396039603960396</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="12">
         <v>0.1</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="13">
         <v>4.1666666666666602E-2</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="14">
         <v>7.8125E-2</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="12">
         <v>0.38461538461538403</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="13">
         <v>0.14705882352941099</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="14">
         <v>0.290697674418604</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="12">
         <v>0.41666666666666602</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="13">
         <v>0.116279069767441</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="14">
         <v>0.27472527472527403</v>
       </c>
-      <c r="R8" s="15">
+      <c r="R8" s="12">
         <v>0.25</v>
       </c>
-      <c r="S8" s="16">
+      <c r="S8" s="13">
         <v>0.12</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="14">
         <v>0.20547945205479401</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U8" s="12">
         <v>0.33333333333333298</v>
       </c>
-      <c r="V8" s="16">
+      <c r="V8" s="13">
         <v>0.13793103448275801</v>
       </c>
-      <c r="W8" s="17">
+      <c r="W8" s="14">
         <v>0.25974025974025899</v>
       </c>
-      <c r="X8" s="15">
+      <c r="X8" s="12">
         <v>0.1</v>
       </c>
-      <c r="Y8" s="16">
+      <c r="Y8" s="13">
         <v>4.3478260869565202E-2</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="Z8" s="14">
         <v>7.9365079365079305E-2</v>
       </c>
-      <c r="AA8" s="18">
+      <c r="AA8" s="15">
         <v>0.33333333333333298</v>
       </c>
-      <c r="AB8" s="18">
+      <c r="AB8" s="15">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AC8" s="18">
+      <c r="AC8" s="15">
         <v>0.28571428571428498</v>
       </c>
-      <c r="AD8" s="15">
+      <c r="AD8" s="12">
         <v>0.27272727272727199</v>
       </c>
-      <c r="AE8" s="16">
+      <c r="AE8" s="13">
         <v>0.14285714285714199</v>
       </c>
-      <c r="AF8" s="17">
+      <c r="AF8" s="14">
         <v>0.23076923076923</v>
       </c>
     </row>
@@ -1567,256 +1567,256 @@
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>0.5</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>0.20588235294117599</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>0.38888888888888801</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="12">
         <v>0.46666666666666601</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="13">
         <v>0.194444444444444</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="14">
         <v>0.36458333333333298</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="12">
         <v>0.1</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="13">
         <v>0.05</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="14">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="12">
         <v>0.38461538461538403</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="13">
         <v>0.17241379310344801</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="14">
         <v>0.30864197530864201</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="12">
         <v>0.41666666666666602</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="13">
         <v>0.13157894736842099</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="14">
         <v>0.290697674418604</v>
       </c>
-      <c r="R9" s="15">
+      <c r="R9" s="12">
         <v>0.25</v>
       </c>
-      <c r="S9" s="16">
+      <c r="S9" s="13">
         <v>0.13636363636363599</v>
       </c>
-      <c r="T9" s="17">
+      <c r="T9" s="14">
         <v>0.214285714285714</v>
       </c>
-      <c r="U9" s="15">
+      <c r="U9" s="12">
         <v>0.27272727272727199</v>
       </c>
-      <c r="V9" s="16">
+      <c r="V9" s="13">
         <v>0.13636363636363599</v>
       </c>
-      <c r="W9" s="17">
+      <c r="W9" s="14">
         <v>0.22727272727272699</v>
       </c>
-      <c r="X9" s="15">
+      <c r="X9" s="12">
         <v>0.1</v>
       </c>
-      <c r="Y9" s="16">
+      <c r="Y9" s="13">
         <v>5.2631578947368397E-2</v>
       </c>
-      <c r="Z9" s="17">
+      <c r="Z9" s="14">
         <v>8.4745762711864403E-2</v>
       </c>
-      <c r="AA9" s="18">
+      <c r="AA9" s="15">
         <v>0.33333333333333298</v>
       </c>
-      <c r="AB9" s="18">
+      <c r="AB9" s="15">
         <v>0.25</v>
       </c>
-      <c r="AC9" s="18">
+      <c r="AC9" s="15">
         <v>0.3125</v>
       </c>
-      <c r="AD9" s="15">
+      <c r="AD9" s="12">
         <v>0.27272727272727199</v>
       </c>
-      <c r="AE9" s="16">
+      <c r="AE9" s="13">
         <v>0.1875</v>
       </c>
-      <c r="AF9" s="17">
+      <c r="AF9" s="14">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="17"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="17"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="14"/>
     </row>
-    <row r="11" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="19"/>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="21"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="18"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>0.5</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <v>0.20833333333333301</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <v>0.25</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="13">
         <v>1</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="14">
         <v>0.29411764705882298</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="13">
         <v>0.5</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="14">
         <v>0.20833333333333301</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="13">
         <v>0.66666666666666596</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="14">
         <v>0.21276595744680801</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="12">
         <v>0.1</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="13">
         <v>0.5</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="Q12" s="14">
         <v>0.119047619047619</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="12">
         <v>0.25</v>
       </c>
-      <c r="S12" s="16">
+      <c r="S12" s="13">
         <v>1</v>
       </c>
-      <c r="T12" s="17">
+      <c r="T12" s="14">
         <v>0.29411764705882298</v>
       </c>
-      <c r="U12" s="15">
+      <c r="U12" s="12">
         <v>0.30769230769230699</v>
       </c>
-      <c r="V12" s="16">
+      <c r="V12" s="13">
         <v>0.8</v>
       </c>
-      <c r="W12" s="17">
+      <c r="W12" s="14">
         <v>0.35087719298245601</v>
       </c>
-      <c r="X12" s="15">
+      <c r="X12" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="Y12" s="16">
+      <c r="Y12" s="13">
         <v>0.66666666666666596</v>
       </c>
-      <c r="Z12" s="17">
+      <c r="Z12" s="14">
         <v>0.21276595744680801</v>
       </c>
-      <c r="AA12" s="18">
+      <c r="AA12" s="15">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AB12" s="18">
+      <c r="AB12" s="15">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AC12" s="18">
+      <c r="AC12" s="15">
         <v>0.21276595744680801</v>
       </c>
-      <c r="AD12" s="15">
+      <c r="AD12" s="12">
         <v>0.18181818181818099</v>
       </c>
-      <c r="AE12" s="16">
+      <c r="AE12" s="13">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AF12" s="17">
+      <c r="AF12" s="14">
         <v>0.21276595744680801</v>
       </c>
     </row>
@@ -1824,94 +1824,94 @@
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>0.64285714285714202</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="13">
         <v>0.160714285714285</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>0.40178571428571402</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <v>0.71428571428571397</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="13">
         <v>0.169491525423728</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="14">
         <v>0.434782608695652</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="12">
         <v>0.75</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="13">
         <v>0.219512195121951</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="14">
         <v>0.50561797752808901</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="12">
         <v>0.6</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="13">
         <v>0.183673469387755</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="14">
         <v>0.41284403669724701</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="12">
         <v>0.88888888888888795</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="13">
         <v>0.19277108433734899</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="14">
         <v>0.51612903225806395</v>
       </c>
-      <c r="R13" s="15">
+      <c r="R13" s="12">
         <v>0.6</v>
       </c>
-      <c r="S13" s="16">
+      <c r="S13" s="13">
         <v>0.219512195121951</v>
       </c>
-      <c r="T13" s="17">
+      <c r="T13" s="14">
         <v>0.445544554455445</v>
       </c>
-      <c r="U13" s="15">
+      <c r="U13" s="12">
         <v>0.6875</v>
       </c>
-      <c r="V13" s="16">
+      <c r="V13" s="13">
         <v>0.25</v>
       </c>
-      <c r="W13" s="17">
+      <c r="W13" s="14">
         <v>0.50925925925925897</v>
       </c>
-      <c r="X13" s="15">
+      <c r="X13" s="12">
         <v>0.66666666666666596</v>
       </c>
-      <c r="Y13" s="16">
+      <c r="Y13" s="13">
         <v>0.22727272727272699</v>
       </c>
-      <c r="Z13" s="17">
+      <c r="Z13" s="14">
         <v>0.48076923076923</v>
       </c>
-      <c r="AA13" s="18">
+      <c r="AA13" s="15">
         <v>0.64285714285714202</v>
       </c>
-      <c r="AB13" s="18">
+      <c r="AB13" s="15">
         <v>0.27272727272727199</v>
       </c>
-      <c r="AC13" s="18">
+      <c r="AC13" s="15">
         <v>0.50561797752808901</v>
       </c>
-      <c r="AD13" s="15">
+      <c r="AD13" s="12">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AE13" s="16">
+      <c r="AE13" s="13">
         <v>0.30303030303030298</v>
       </c>
-      <c r="AF13" s="17">
+      <c r="AF13" s="14">
         <v>0.53763440860214995</v>
       </c>
     </row>
@@ -1919,94 +1919,94 @@
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>0.83333333333333304</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>0.22727272727272699</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="14">
         <v>0.54347826086956497</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>0.84210526315789402</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="13">
         <v>0.23880597014925301</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="14">
         <v>0.55944055944055904</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="12">
         <v>0.64285714285714202</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="13">
         <v>0.19565217391304299</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="14">
         <v>0.441176470588235</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="12">
         <v>0.88235294117647001</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="13">
         <v>0.26785714285714202</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="14">
         <v>0.60483870967741904</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O14" s="12">
         <v>0.73684210526315697</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="13">
         <v>0.18181818181818099</v>
       </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="14">
         <v>0.45751633986928097</v>
       </c>
-      <c r="R14" s="15">
+      <c r="R14" s="12">
         <v>0.85</v>
       </c>
-      <c r="S14" s="16">
+      <c r="S14" s="13">
         <v>0.27868852459016302</v>
       </c>
-      <c r="T14" s="17">
+      <c r="T14" s="14">
         <v>0.60283687943262398</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U14" s="12">
         <v>0.84210526315789402</v>
       </c>
-      <c r="V14" s="16">
+      <c r="V14" s="13">
         <v>0.266666666666666</v>
       </c>
-      <c r="W14" s="17">
+      <c r="W14" s="14">
         <v>0.58823529411764697</v>
       </c>
-      <c r="X14" s="15">
+      <c r="X14" s="12">
         <v>0.8</v>
       </c>
-      <c r="Y14" s="16">
+      <c r="Y14" s="13">
         <v>0.25</v>
       </c>
-      <c r="Z14" s="17">
+      <c r="Z14" s="14">
         <v>0.55555555555555503</v>
       </c>
-      <c r="AA14" s="18">
+      <c r="AA14" s="15">
         <v>0.83333333333333304</v>
       </c>
-      <c r="AB14" s="18">
+      <c r="AB14" s="15">
         <v>0.29411764705882298</v>
       </c>
-      <c r="AC14" s="18">
+      <c r="AC14" s="15">
         <v>0.60975609756097504</v>
       </c>
-      <c r="AD14" s="15">
+      <c r="AD14" s="12">
         <v>0.8125</v>
       </c>
-      <c r="AE14" s="16">
+      <c r="AE14" s="13">
         <v>0.26</v>
       </c>
-      <c r="AF14" s="17">
+      <c r="AF14" s="14">
         <v>0.570175438596491</v>
       </c>
     </row>
@@ -2014,94 +2014,94 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>0.75</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>0.241935483870967</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="14">
         <v>0.528169014084507</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="12">
         <v>0.8</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="13">
         <v>0.231884057971014</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="14">
         <v>0.53691275167785202</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="12">
         <v>0.82352941176470495</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="13">
         <v>0.27450980392156799</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="14">
         <v>0.58823529411764697</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="12">
         <v>0.90476190476190399</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="13">
         <v>0.29230769230769199</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="14">
         <v>0.63758389261744897</v>
       </c>
-      <c r="O15" s="15">
+      <c r="O15" s="12">
         <v>0.77777777777777701</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="13">
         <v>0.19178082191780799</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="14">
         <v>0.48275862068965503</v>
       </c>
-      <c r="R15" s="15">
+      <c r="R15" s="12">
         <v>0.85</v>
       </c>
-      <c r="S15" s="16">
+      <c r="S15" s="13">
         <v>0.32692307692307598</v>
       </c>
-      <c r="T15" s="17">
+      <c r="T15" s="14">
         <v>0.64393939393939303</v>
       </c>
-      <c r="U15" s="15">
+      <c r="U15" s="12">
         <v>0.90909090909090895</v>
       </c>
-      <c r="V15" s="16">
+      <c r="V15" s="13">
         <v>0.32258064516128998</v>
       </c>
-      <c r="W15" s="17">
+      <c r="W15" s="14">
         <v>0.66666666666666596</v>
       </c>
-      <c r="X15" s="15">
+      <c r="X15" s="12">
         <v>0.78947368421052599</v>
       </c>
-      <c r="Y15" s="16">
+      <c r="Y15" s="13">
         <v>0.28846153846153799</v>
       </c>
-      <c r="Z15" s="17">
+      <c r="Z15" s="14">
         <v>0.5859375</v>
       </c>
-      <c r="AA15" s="18">
+      <c r="AA15" s="15">
         <v>0.85714285714285698</v>
       </c>
-      <c r="AB15" s="18">
+      <c r="AB15" s="15">
         <v>0.34615384615384598</v>
       </c>
-      <c r="AC15" s="18">
+      <c r="AC15" s="15">
         <v>0.66176470588235203</v>
       </c>
-      <c r="AD15" s="15">
+      <c r="AD15" s="12">
         <v>0.9</v>
       </c>
-      <c r="AE15" s="16">
+      <c r="AE15" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="AF15" s="17">
+      <c r="AF15" s="14">
         <v>0.67164179104477595</v>
       </c>
     </row>
@@ -2109,163 +2109,163 @@
       <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>0.73684210526315697</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="13">
         <v>0.22222222222222199</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="14">
         <v>0.50359712230215803</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="12">
         <v>0.85</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="13">
         <v>0.23943661971830901</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="14">
         <v>0.56291390728476798</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="12">
         <v>0.8</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="13">
         <v>0.24489795918367299</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="14">
         <v>0.55045871559632997</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="12">
         <v>0.9</v>
       </c>
-      <c r="M16" s="16">
+      <c r="M16" s="13">
         <v>0.3</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="14">
         <v>0.64285714285714202</v>
       </c>
-      <c r="O16" s="15">
+      <c r="O16" s="12">
         <v>0.72222222222222199</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16" s="13">
         <v>0.17567567567567499</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="14">
         <v>0.44520547945205402</v>
       </c>
-      <c r="R16" s="15">
+      <c r="R16" s="12">
         <v>0.77777777777777701</v>
       </c>
-      <c r="S16" s="16">
+      <c r="S16" s="13">
         <v>0.28571428571428498</v>
       </c>
-      <c r="T16" s="17">
+      <c r="T16" s="14">
         <v>0.57851239669421395</v>
       </c>
-      <c r="U16" s="15">
+      <c r="U16" s="12">
         <v>0.84210526315789402</v>
       </c>
-      <c r="V16" s="16">
+      <c r="V16" s="13">
         <v>0.27118644067796599</v>
       </c>
-      <c r="W16" s="17">
+      <c r="W16" s="14">
         <v>0.592592592592592</v>
       </c>
-      <c r="X16" s="15">
+      <c r="X16" s="12">
         <v>0.6875</v>
       </c>
-      <c r="Y16" s="16">
+      <c r="Y16" s="13">
         <v>0.22448979591836701</v>
       </c>
-      <c r="Z16" s="17">
+      <c r="Z16" s="14">
         <v>0.48672566371681403</v>
       </c>
-      <c r="AA16" s="18">
+      <c r="AA16" s="15">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AB16" s="18">
+      <c r="AB16" s="15">
         <v>0.3</v>
       </c>
-      <c r="AC16" s="18">
+      <c r="AC16" s="15">
         <v>0.59523809523809501</v>
       </c>
-      <c r="AD16" s="15">
+      <c r="AD16" s="12">
         <v>0.77777777777777701</v>
       </c>
-      <c r="AE16" s="16">
+      <c r="AE16" s="13">
         <v>0.29166666666666602</v>
       </c>
-      <c r="AF16" s="17">
+      <c r="AF16" s="14">
         <v>0.58333333333333304</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="16"/>
-      <c r="AF17" s="17"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="14"/>
     </row>
-    <row r="18" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="20"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="19"/>
-      <c r="AE18" s="20"/>
-      <c r="AF18" s="21"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="18"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="18"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -2274,7 +2274,7 @@
       <c r="C19" s="1">
         <v>0.75</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="20">
         <v>0.483870967741935</v>
       </c>
       <c r="E19" s="3">
@@ -2283,7 +2283,7 @@
       <c r="F19" s="1">
         <v>0.625</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="20">
         <v>0.37037037037037002</v>
       </c>
       <c r="H19" s="3">
@@ -2292,7 +2292,7 @@
       <c r="I19" s="1">
         <v>0.72222222222222199</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="20">
         <v>0.44827586206896503</v>
       </c>
       <c r="K19" s="3">
@@ -2301,7 +2301,7 @@
       <c r="L19" s="1">
         <v>0.77777777777777701</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M19" s="20">
         <v>0.46666666666666601</v>
       </c>
       <c r="N19" s="3">
@@ -2310,7 +2310,7 @@
       <c r="O19" s="1">
         <v>0.75</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P19" s="20">
         <v>0.46875</v>
       </c>
       <c r="Q19" s="3">
@@ -2319,7 +2319,7 @@
       <c r="R19" s="1">
         <v>0.70588235294117596</v>
       </c>
-      <c r="S19" s="23">
+      <c r="S19" s="20">
         <v>0.375</v>
       </c>
       <c r="T19" s="3">
@@ -2328,7 +2328,7 @@
       <c r="U19" s="1">
         <v>0.625</v>
       </c>
-      <c r="V19" s="23">
+      <c r="V19" s="20">
         <v>0.30303030303030298</v>
       </c>
       <c r="W19" s="3">
@@ -2337,7 +2337,7 @@
       <c r="X19" s="1">
         <v>0.72222222222222199</v>
       </c>
-      <c r="Y19" s="23">
+      <c r="Y19" s="20">
         <v>0.43333333333333302</v>
       </c>
       <c r="Z19" s="3">
@@ -2355,7 +2355,7 @@
       <c r="AD19" s="1">
         <v>0.70588235294117596</v>
       </c>
-      <c r="AE19" s="23">
+      <c r="AE19" s="20">
         <v>0.375</v>
       </c>
       <c r="AF19" s="3">
@@ -2366,94 +2366,94 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="12">
         <v>0.76470588235294101</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>0.36111111111111099</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="14">
         <v>0.625</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="12">
         <v>0.70588235294117596</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="13">
         <v>0.34285714285714203</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="14">
         <v>0.58252427184466005</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="12">
         <v>0.83333333333333304</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="13">
         <v>0.45454545454545398</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="14">
         <v>0.71428571428571397</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="12">
         <v>0.85</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="13">
         <v>0.44736842105263103</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="14">
         <v>0.72033898305084698</v>
       </c>
-      <c r="O20" s="15">
+      <c r="O20" s="12">
         <v>0.625</v>
       </c>
-      <c r="P20" s="16">
+      <c r="P20" s="13">
         <v>0.238095238095238</v>
       </c>
-      <c r="Q20" s="17">
+      <c r="Q20" s="14">
         <v>0.47169811320754701</v>
       </c>
-      <c r="R20" s="15">
+      <c r="R20" s="12">
         <v>0.70588235294117596</v>
       </c>
-      <c r="S20" s="16">
+      <c r="S20" s="13">
         <v>0.4</v>
       </c>
-      <c r="T20" s="17">
+      <c r="T20" s="14">
         <v>0.61224489795918302</v>
       </c>
-      <c r="U20" s="15">
+      <c r="U20" s="12">
         <v>0.85</v>
       </c>
-      <c r="V20" s="16">
+      <c r="V20" s="13">
         <v>0.48571428571428499</v>
       </c>
-      <c r="W20" s="17">
+      <c r="W20" s="14">
         <v>0.73913043478260798</v>
       </c>
-      <c r="X20" s="15">
+      <c r="X20" s="12">
         <v>0.75</v>
       </c>
-      <c r="Y20" s="16">
+      <c r="Y20" s="13">
         <v>0.46875</v>
       </c>
-      <c r="Z20" s="17">
+      <c r="Z20" s="14">
         <v>0.66964285714285698</v>
       </c>
-      <c r="AA20" s="18">
+      <c r="AA20" s="15">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AB20" s="18">
+      <c r="AB20" s="15">
         <v>0.42857142857142799</v>
       </c>
-      <c r="AC20" s="18">
+      <c r="AC20" s="15">
         <v>0.67567567567567499</v>
       </c>
-      <c r="AD20" s="15">
+      <c r="AD20" s="12">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AE20" s="16">
+      <c r="AE20" s="13">
         <v>0.46875</v>
       </c>
-      <c r="AF20" s="17">
+      <c r="AF20" s="14">
         <v>0.69444444444444398</v>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
       <c r="C21" s="1">
         <v>0.8</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="20">
         <v>0.36363636363636298</v>
       </c>
       <c r="E21" s="3">
@@ -2473,7 +2473,7 @@
       <c r="F21" s="1">
         <v>0.76190476190476097</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="20">
         <v>0.35555555555555501</v>
       </c>
       <c r="H21" s="3">
@@ -2482,7 +2482,7 @@
       <c r="I21" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21" s="20">
         <v>0.36585365853658502</v>
       </c>
       <c r="K21" s="3">
@@ -2491,7 +2491,7 @@
       <c r="L21" s="1">
         <v>0.86363636363636298</v>
       </c>
-      <c r="M21" s="23">
+      <c r="M21" s="20">
         <v>0.47499999999999998</v>
       </c>
       <c r="N21" s="3">
@@ -2500,7 +2500,7 @@
       <c r="O21" s="1">
         <v>0.64705882352941102</v>
       </c>
-      <c r="P21" s="23">
+      <c r="P21" s="20">
         <v>0.23913043478260801</v>
       </c>
       <c r="Q21" s="3">
@@ -2509,7 +2509,7 @@
       <c r="R21" s="1">
         <v>0.78947368421052599</v>
       </c>
-      <c r="S21" s="23">
+      <c r="S21" s="20">
         <v>0.41666666666666602</v>
       </c>
       <c r="T21" s="3">
@@ -2518,7 +2518,7 @@
       <c r="U21" s="1">
         <v>0.85</v>
       </c>
-      <c r="V21" s="23">
+      <c r="V21" s="20">
         <v>0.42499999999999999</v>
       </c>
       <c r="W21" s="3">
@@ -2527,7 +2527,7 @@
       <c r="X21" s="1">
         <v>0.77777777777777701</v>
       </c>
-      <c r="Y21" s="23">
+      <c r="Y21" s="20">
         <v>0.38888888888888801</v>
       </c>
       <c r="Z21" s="3">
@@ -2545,7 +2545,7 @@
       <c r="AD21" s="1">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AE21" s="23">
+      <c r="AE21" s="20">
         <v>0.394736842105263</v>
       </c>
       <c r="AF21" s="3">
@@ -2559,7 +2559,7 @@
       <c r="C22" s="1">
         <v>0.8</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="20">
         <v>0.36363636363636298</v>
       </c>
       <c r="E22" s="3">
@@ -2568,7 +2568,7 @@
       <c r="F22" s="1">
         <v>0.76190476190476097</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="20">
         <v>0.35555555555555501</v>
       </c>
       <c r="H22" s="3">
@@ -2577,7 +2577,7 @@
       <c r="I22" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="20">
         <v>0.36585365853658502</v>
       </c>
       <c r="K22" s="3">
@@ -2586,7 +2586,7 @@
       <c r="L22" s="1">
         <v>0.86363636363636298</v>
       </c>
-      <c r="M22" s="23">
+      <c r="M22" s="20">
         <v>0.47499999999999998</v>
       </c>
       <c r="N22" s="3">
@@ -2595,7 +2595,7 @@
       <c r="O22" s="1">
         <v>0.64705882352941102</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="20">
         <v>0.23913043478260801</v>
       </c>
       <c r="Q22" s="3">
@@ -2604,7 +2604,7 @@
       <c r="R22" s="1">
         <v>0.78947368421052599</v>
       </c>
-      <c r="S22" s="23">
+      <c r="S22" s="20">
         <v>0.41666666666666602</v>
       </c>
       <c r="T22" s="3">
@@ -2613,7 +2613,7 @@
       <c r="U22" s="1">
         <v>0.85</v>
       </c>
-      <c r="V22" s="23">
+      <c r="V22" s="20">
         <v>0.42499999999999999</v>
       </c>
       <c r="W22" s="3">
@@ -2622,7 +2622,7 @@
       <c r="X22" s="1">
         <v>0.77777777777777701</v>
       </c>
-      <c r="Y22" s="23">
+      <c r="Y22" s="20">
         <v>0.38888888888888801</v>
       </c>
       <c r="Z22" s="3">
@@ -2640,7 +2640,7 @@
       <c r="AD22" s="1">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AE22" s="23">
+      <c r="AE22" s="20">
         <v>0.394736842105263</v>
       </c>
       <c r="AF22" s="3">
@@ -2654,7 +2654,7 @@
       <c r="C23" s="1">
         <v>0.8</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="20">
         <v>0.36363636363636298</v>
       </c>
       <c r="E23" s="3">
@@ -2663,7 +2663,7 @@
       <c r="F23" s="1">
         <v>0.76190476190476097</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="20">
         <v>0.35555555555555501</v>
       </c>
       <c r="H23" s="3">
@@ -2672,7 +2672,7 @@
       <c r="I23" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="20">
         <v>0.36585365853658502</v>
       </c>
       <c r="K23" s="3">
@@ -2681,7 +2681,7 @@
       <c r="L23" s="1">
         <v>0.86363636363636298</v>
       </c>
-      <c r="M23" s="23">
+      <c r="M23" s="20">
         <v>0.47499999999999998</v>
       </c>
       <c r="N23" s="3">
@@ -2690,7 +2690,7 @@
       <c r="O23" s="1">
         <v>0.64705882352941102</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="20">
         <v>0.23913043478260801</v>
       </c>
       <c r="Q23" s="3">
@@ -2699,7 +2699,7 @@
       <c r="R23" s="1">
         <v>0.78947368421052599</v>
       </c>
-      <c r="S23" s="23">
+      <c r="S23" s="20">
         <v>0.41666666666666602</v>
       </c>
       <c r="T23" s="3">
@@ -2708,7 +2708,7 @@
       <c r="U23" s="1">
         <v>0.85</v>
       </c>
-      <c r="V23" s="23">
+      <c r="V23" s="20">
         <v>0.42499999999999999</v>
       </c>
       <c r="W23" s="3">
@@ -2717,7 +2717,7 @@
       <c r="X23" s="1">
         <v>0.77777777777777701</v>
       </c>
-      <c r="Y23" s="23">
+      <c r="Y23" s="20">
         <v>0.38888888888888801</v>
       </c>
       <c r="Z23" s="3">
@@ -2735,7 +2735,7 @@
       <c r="AD23" s="1">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AE23" s="23">
+      <c r="AE23" s="20">
         <v>0.394736842105263</v>
       </c>
       <c r="AF23" s="3">
@@ -2743,164 +2743,164 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="18"/>
-      <c r="AB24" s="18"/>
-      <c r="AC24" s="18"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="16"/>
-      <c r="AF24" s="17"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="12"/>
+      <c r="AE24" s="13"/>
+      <c r="AF24" s="14"/>
     </row>
-    <row r="25" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="20"/>
-      <c r="W25" s="21"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="20"/>
-      <c r="Z25" s="21"/>
-      <c r="AA25" s="22"/>
-      <c r="AB25" s="22"/>
-      <c r="AC25" s="22"/>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="20"/>
-      <c r="AF25" s="21"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="16"/>
+      <c r="AE25" s="17"/>
+      <c r="AF25" s="18"/>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="12">
         <v>0.6875</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="13">
         <v>0.39285714285714202</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="14">
         <v>0.59782608695652095</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="12">
         <v>0.66666666666666596</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="13">
         <v>0.44444444444444398</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="14">
         <v>0.60606060606060597</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="12">
         <v>0.66666666666666596</v>
       </c>
-      <c r="J26" s="16">
+      <c r="J26" s="13">
         <v>0.35714285714285698</v>
       </c>
-      <c r="K26" s="17">
+      <c r="K26" s="14">
         <v>0.56818181818181801</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="12">
         <v>0.66666666666666596</v>
       </c>
-      <c r="M26" s="16">
+      <c r="M26" s="13">
         <v>0.38461538461538403</v>
       </c>
-      <c r="N26" s="17">
+      <c r="N26" s="14">
         <v>0.581395348837209</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="12">
         <v>0.73684210526315697</v>
       </c>
-      <c r="P26" s="16">
+      <c r="P26" s="13">
         <v>0.45161290322580599</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="14">
         <v>0.65420560747663503</v>
       </c>
-      <c r="R26" s="15">
+      <c r="R26" s="12">
         <v>0.6875</v>
       </c>
-      <c r="S26" s="16">
+      <c r="S26" s="13">
         <v>0.407407407407407</v>
       </c>
-      <c r="T26" s="17">
+      <c r="T26" s="14">
         <v>0.60439560439560402</v>
       </c>
-      <c r="U26" s="15">
+      <c r="U26" s="12">
         <v>0.625</v>
       </c>
-      <c r="V26" s="16">
+      <c r="V26" s="13">
         <v>0.30303030303030298</v>
       </c>
-      <c r="W26" s="17">
+      <c r="W26" s="14">
         <v>0.51546391752577303</v>
       </c>
-      <c r="X26" s="15">
+      <c r="X26" s="12">
         <v>0.6875</v>
       </c>
-      <c r="Y26" s="16">
+      <c r="Y26" s="13">
         <v>0.39285714285714202</v>
       </c>
-      <c r="Z26" s="17">
+      <c r="Z26" s="14">
         <v>0.59782608695652095</v>
       </c>
-      <c r="AA26" s="18">
+      <c r="AA26" s="15">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AB26" s="18">
+      <c r="AB26" s="15">
         <v>0.33333333333333298</v>
       </c>
-      <c r="AC26" s="18">
+      <c r="AC26" s="15">
         <v>0.55555555555555503</v>
       </c>
-      <c r="AD26" s="15">
+      <c r="AD26" s="12">
         <v>0.66666666666666596</v>
       </c>
-      <c r="AE26" s="16">
+      <c r="AE26" s="13">
         <v>0.34482758620689602</v>
       </c>
-      <c r="AF26" s="17">
+      <c r="AF26" s="14">
         <v>0.56179775280898803</v>
       </c>
     </row>
@@ -2908,94 +2908,94 @@
       <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="12">
         <v>0.76470588235294101</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="13">
         <v>0.27659574468085102</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="14">
         <v>0.56521739130434701</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="12">
         <v>0.70588235294117596</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="13">
         <v>0.26086956521739102</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H27" s="14">
         <v>0.52631578947368396</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="12">
         <v>0.88888888888888795</v>
       </c>
-      <c r="J27" s="16">
+      <c r="J27" s="13">
         <v>0.372093023255814</v>
       </c>
-      <c r="K27" s="17">
+      <c r="K27" s="14">
         <v>0.69565217391304301</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="12">
         <v>0.84210526315789402</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27" s="13">
         <v>0.36363636363636298</v>
       </c>
-      <c r="N27" s="17">
+      <c r="N27" s="14">
         <v>0.66666666666666596</v>
       </c>
-      <c r="O27" s="15">
+      <c r="O27" s="12">
         <v>0.6875</v>
       </c>
-      <c r="P27" s="16">
+      <c r="P27" s="13">
         <v>0.19642857142857101</v>
       </c>
-      <c r="Q27" s="17">
+      <c r="Q27" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="R27" s="15">
+      <c r="R27" s="12">
         <v>0.76470588235294101</v>
       </c>
-      <c r="S27" s="16">
+      <c r="S27" s="13">
         <v>0.36111111111111099</v>
       </c>
-      <c r="T27" s="17">
+      <c r="T27" s="14">
         <v>0.625</v>
       </c>
-      <c r="U27" s="15">
+      <c r="U27" s="12">
         <v>0.9</v>
       </c>
-      <c r="V27" s="16">
+      <c r="V27" s="13">
         <v>0.4</v>
       </c>
-      <c r="W27" s="17">
+      <c r="W27" s="14">
         <v>0.72</v>
       </c>
-      <c r="X27" s="15">
+      <c r="X27" s="12">
         <v>0.75</v>
       </c>
-      <c r="Y27" s="16">
+      <c r="Y27" s="13">
         <v>0.40540540540540498</v>
       </c>
-      <c r="Z27" s="17">
+      <c r="Z27" s="14">
         <v>0.64102564102564097</v>
       </c>
-      <c r="AA27" s="18">
+      <c r="AA27" s="15">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AB27" s="18">
+      <c r="AB27" s="15">
         <v>0.36585365853658502</v>
       </c>
-      <c r="AC27" s="18">
+      <c r="AC27" s="15">
         <v>0.64102564102564097</v>
       </c>
-      <c r="AD27" s="15">
+      <c r="AD27" s="12">
         <v>0.78947368421052599</v>
       </c>
-      <c r="AE27" s="16">
+      <c r="AE27" s="13">
         <v>0.394736842105263</v>
       </c>
-      <c r="AF27" s="17">
+      <c r="AF27" s="14">
         <v>0.65789473684210498</v>
       </c>
     </row>
@@ -3006,7 +3006,7 @@
       <c r="C28" s="1">
         <v>0.85714285714285698</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="20">
         <v>0.33333333333333298</v>
       </c>
       <c r="E28" s="3">
@@ -3015,7 +3015,7 @@
       <c r="F28" s="1">
         <v>0.80952380952380898</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="20">
         <v>0.29310344827586199</v>
       </c>
       <c r="H28" s="3">
@@ -3024,7 +3024,7 @@
       <c r="I28" s="1">
         <v>0.89473684210526305</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J28" s="20">
         <v>0.33333333333333298</v>
       </c>
       <c r="K28" s="3">
@@ -3033,7 +3033,7 @@
       <c r="L28" s="1">
         <v>0.91304347826086896</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="20">
         <v>0.41176470588235198</v>
       </c>
       <c r="N28" s="3">
@@ -3042,7 +3042,7 @@
       <c r="O28" s="1">
         <v>0.70588235294117596</v>
       </c>
-      <c r="P28" s="23">
+      <c r="P28" s="20">
         <v>0.19047619047618999</v>
       </c>
       <c r="Q28" s="3">
@@ -3051,7 +3051,7 @@
       <c r="R28" s="1">
         <v>0.85</v>
       </c>
-      <c r="S28" s="23">
+      <c r="S28" s="20">
         <v>0.36956521739130399</v>
       </c>
       <c r="T28" s="3">
@@ -3060,7 +3060,7 @@
       <c r="U28" s="1">
         <v>0.90476190476190399</v>
       </c>
-      <c r="V28" s="23">
+      <c r="V28" s="20">
         <v>0.35849056603773499</v>
       </c>
       <c r="W28" s="3">
@@ -3069,7 +3069,7 @@
       <c r="X28" s="1">
         <v>0.85</v>
       </c>
-      <c r="Y28" s="23">
+      <c r="Y28" s="20">
         <v>0.36170212765957399</v>
       </c>
       <c r="Z28" s="3">
@@ -3087,7 +3087,7 @@
       <c r="AD28" s="1">
         <v>0.85</v>
       </c>
-      <c r="AE28" s="23">
+      <c r="AE28" s="20">
         <v>0.35416666666666602</v>
       </c>
       <c r="AF28" s="3">
@@ -3098,94 +3098,94 @@
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="12">
         <v>0.8</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="13">
         <v>0.30769230769230699</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="14">
         <v>0.60606060606060597</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="12">
         <v>0.80952380952380898</v>
       </c>
-      <c r="G29" s="16">
+      <c r="G29" s="13">
         <v>0.28813559322033899</v>
       </c>
-      <c r="H29" s="17">
+      <c r="H29" s="14">
         <v>0.59440559440559404</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="12">
         <v>0.88888888888888795</v>
       </c>
-      <c r="J29" s="16">
+      <c r="J29" s="13">
         <v>0.32</v>
       </c>
-      <c r="K29" s="17">
+      <c r="K29" s="14">
         <v>0.65573770491803196</v>
       </c>
-      <c r="L29" s="15">
+      <c r="L29" s="12">
         <v>0.91304347826086896</v>
       </c>
-      <c r="M29" s="16">
+      <c r="M29" s="13">
         <v>0.41176470588235198</v>
       </c>
-      <c r="N29" s="17">
+      <c r="N29" s="14">
         <v>0.73426573426573405</v>
       </c>
-      <c r="O29" s="15">
+      <c r="O29" s="12">
         <v>0.70588235294117596</v>
       </c>
-      <c r="P29" s="16">
+      <c r="P29" s="13">
         <v>0.19354838709677399</v>
       </c>
-      <c r="Q29" s="17">
+      <c r="Q29" s="14">
         <v>0.46153846153846101</v>
       </c>
-      <c r="R29" s="15">
+      <c r="R29" s="12">
         <v>0.85</v>
       </c>
-      <c r="S29" s="16">
+      <c r="S29" s="13">
         <v>0.36956521739130399</v>
       </c>
-      <c r="T29" s="17">
+      <c r="T29" s="14">
         <v>0.67460317460317398</v>
       </c>
-      <c r="U29" s="15">
+      <c r="U29" s="12">
         <v>0.9</v>
       </c>
-      <c r="V29" s="16">
+      <c r="V29" s="13">
         <v>0.36</v>
       </c>
-      <c r="W29" s="17">
+      <c r="W29" s="14">
         <v>0.69230769230769196</v>
       </c>
-      <c r="X29" s="15">
+      <c r="X29" s="12">
         <v>0.83333333333333304</v>
       </c>
-      <c r="Y29" s="16">
+      <c r="Y29" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="Z29" s="17">
+      <c r="Z29" s="14">
         <v>0.64102564102564097</v>
       </c>
-      <c r="AA29" s="18">
+      <c r="AA29" s="15">
         <v>0.85</v>
       </c>
-      <c r="AB29" s="18">
+      <c r="AB29" s="15">
         <v>0.36170212765957399</v>
       </c>
-      <c r="AC29" s="18">
+      <c r="AC29" s="15">
         <v>0.66929133858267698</v>
       </c>
-      <c r="AD29" s="15">
+      <c r="AD29" s="12">
         <v>0.84210526315789402</v>
       </c>
-      <c r="AE29" s="16">
+      <c r="AE29" s="13">
         <v>0.340425531914893</v>
       </c>
-      <c r="AF29" s="17">
+      <c r="AF29" s="14">
         <v>0.65040650406503997</v>
       </c>
     </row>
@@ -3193,169 +3193,169 @@
       <c r="B30" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="12">
         <v>0.8</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="13">
         <v>0.30769230769230699</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="14">
         <v>0.60606060606060597</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="12">
         <v>0.80952380952380898</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="13">
         <v>0.28813559322033899</v>
       </c>
-      <c r="H30" s="17">
+      <c r="H30" s="14">
         <v>0.59440559440559404</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="12">
         <v>0.88888888888888795</v>
       </c>
-      <c r="J30" s="16">
+      <c r="J30" s="13">
         <v>0.32</v>
       </c>
-      <c r="K30" s="17">
+      <c r="K30" s="14">
         <v>0.65573770491803196</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="12">
         <v>0.91304347826086896</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="13">
         <v>0.41176470588235198</v>
       </c>
-      <c r="N30" s="17">
+      <c r="N30" s="14">
         <v>0.73426573426573405</v>
       </c>
-      <c r="O30" s="15">
+      <c r="O30" s="12">
         <v>0.70588235294117596</v>
       </c>
-      <c r="P30" s="16">
+      <c r="P30" s="13">
         <v>0.19354838709677399</v>
       </c>
-      <c r="Q30" s="17">
+      <c r="Q30" s="14">
         <v>0.46153846153846101</v>
       </c>
-      <c r="R30" s="15">
+      <c r="R30" s="12">
         <v>0.85</v>
       </c>
-      <c r="S30" s="16">
+      <c r="S30" s="13">
         <v>0.36956521739130399</v>
       </c>
-      <c r="T30" s="17">
+      <c r="T30" s="14">
         <v>0.67460317460317398</v>
       </c>
-      <c r="U30" s="15">
+      <c r="U30" s="12">
         <v>0.9</v>
       </c>
-      <c r="V30" s="16">
+      <c r="V30" s="13">
         <v>0.35294117647058798</v>
       </c>
-      <c r="W30" s="17">
+      <c r="W30" s="14">
         <v>0.68702290076335804</v>
       </c>
-      <c r="X30" s="15">
+      <c r="X30" s="12">
         <v>0.83333333333333304</v>
       </c>
-      <c r="Y30" s="16">
+      <c r="Y30" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="Z30" s="17">
+      <c r="Z30" s="14">
         <v>0.64102564102564097</v>
       </c>
-      <c r="AA30" s="18">
+      <c r="AA30" s="15">
         <v>0.85</v>
       </c>
-      <c r="AB30" s="18">
+      <c r="AB30" s="15">
         <v>0.36170212765957399</v>
       </c>
-      <c r="AC30" s="18">
+      <c r="AC30" s="15">
         <v>0.66929133858267698</v>
       </c>
-      <c r="AD30" s="15">
+      <c r="AD30" s="12">
         <v>0.84210526315789402</v>
       </c>
-      <c r="AE30" s="16">
+      <c r="AE30" s="13">
         <v>0.34782608695652101</v>
       </c>
-      <c r="AF30" s="17">
+      <c r="AF30" s="14">
         <v>0.65573770491803196</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="16"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="18"/>
-      <c r="AB31" s="18"/>
-      <c r="AC31" s="18"/>
-      <c r="AD31" s="15"/>
-      <c r="AE31" s="16"/>
-      <c r="AF31" s="17"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="15"/>
+      <c r="AB31" s="15"/>
+      <c r="AC31" s="15"/>
+      <c r="AD31" s="12"/>
+      <c r="AE31" s="13"/>
+      <c r="AF31" s="14"/>
     </row>
-    <row r="32" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+    <row r="32" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="21"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="20"/>
-      <c r="Z32" s="21"/>
-      <c r="AA32" s="22"/>
-      <c r="AB32" s="22"/>
-      <c r="AC32" s="22"/>
-      <c r="AD32" s="19"/>
-      <c r="AE32" s="20"/>
-      <c r="AF32" s="21"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="16"/>
+      <c r="AE32" s="17"/>
+      <c r="AF32" s="18"/>
     </row>
     <row r="33" spans="3:32" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>0.8</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="20">
         <v>0.25</v>
       </c>
       <c r="E33" s="3">
@@ -3364,7 +3364,7 @@
       <c r="F33" s="1">
         <v>0.80952380952380898</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="20">
         <v>0.24285714285714199</v>
       </c>
       <c r="H33" s="3">
@@ -3373,7 +3373,7 @@
       <c r="I33" s="1">
         <v>0.88888888888888795</v>
       </c>
-      <c r="J33" s="23">
+      <c r="J33" s="20">
         <v>0.30188679245283001</v>
       </c>
       <c r="K33" s="3">
@@ -3382,7 +3382,7 @@
       <c r="L33" s="1">
         <v>0.91304347826086896</v>
       </c>
-      <c r="M33" s="23">
+      <c r="M33" s="20">
         <v>0.328125</v>
       </c>
       <c r="N33" s="3">
@@ -3391,7 +3391,7 @@
       <c r="O33" s="1">
         <v>0.77777777777777701</v>
       </c>
-      <c r="P33" s="23">
+      <c r="P33" s="20">
         <v>0.19178082191780799</v>
       </c>
       <c r="Q33" s="3">
@@ -3400,7 +3400,7 @@
       <c r="R33" s="1">
         <v>0.85</v>
       </c>
-      <c r="S33" s="23">
+      <c r="S33" s="20">
         <v>0.31481481481481399</v>
       </c>
       <c r="T33" s="3">
@@ -3409,7 +3409,7 @@
       <c r="U33" s="1">
         <v>0.9</v>
       </c>
-      <c r="V33" s="23">
+      <c r="V33" s="20">
         <v>0.31578947368421001</v>
       </c>
       <c r="W33" s="3">
@@ -3418,7 +3418,7 @@
       <c r="X33" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="Y33" s="23">
+      <c r="Y33" s="20">
         <v>0.30612244897959101</v>
       </c>
       <c r="Z33" s="3">
@@ -3436,7 +3436,7 @@
       <c r="AD33" s="1">
         <v>0.84210526315789402</v>
       </c>
-      <c r="AE33" s="23">
+      <c r="AE33" s="20">
         <v>0.31372549019607798</v>
       </c>
       <c r="AF33" s="3">
@@ -3445,6 +3445,7 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C2:E2"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AA2:AC2"/>
@@ -3454,7 +3455,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>